<commit_message>
PC: Subiendo las técnicas
</commit_message>
<xml_diff>
--- a/bdd/bdd_acv2.xlsx
+++ b/bdd/bdd_acv2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abraham\Documents\Machine-Learning-con-Jupiter\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D69B19E-32AF-4D00-94B7-3CCAFB476F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949133DC-F56D-405B-B770-8F1CD266044B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="4305" windowWidth="14085" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1695" windowWidth="19095" windowHeight="18090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stroke" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="55">
   <si>
     <t>Hb A/C  %</t>
   </si>
@@ -231,21 +231,6 @@
   </si>
   <si>
     <t>SEX</t>
-  </si>
-  <si>
-    <t>Media</t>
-  </si>
-  <si>
-    <t>Contar no Null</t>
-  </si>
-  <si>
-    <t>Desviación Estándar</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Máx</t>
   </si>
 </sst>
 </file>
@@ -921,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="AQ25" sqref="AQ25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:AQ68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6803,1294 +6788,394 @@
       <c r="AO50" s="11"/>
     </row>
     <row r="51" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="H51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="I51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="J51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="K51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="L51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="M51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="N51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="O51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="P51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="R51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="S51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="T51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="U51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="V51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="W51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="X51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK51" s="25" t="s">
-        <v>56</v>
-      </c>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="25"/>
+      <c r="P51" s="25"/>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="25"/>
+      <c r="S51" s="25"/>
+      <c r="T51" s="25"/>
+      <c r="U51" s="25"/>
+      <c r="V51" s="25"/>
+      <c r="W51" s="25"/>
+      <c r="X51" s="25"/>
+      <c r="Y51" s="25"/>
+      <c r="Z51" s="25"/>
+      <c r="AA51" s="25"/>
+      <c r="AB51" s="25"/>
+      <c r="AC51" s="25"/>
+      <c r="AD51" s="25"/>
+      <c r="AE51" s="25"/>
+      <c r="AF51" s="25"/>
+      <c r="AG51" s="25"/>
+      <c r="AH51" s="25"/>
+      <c r="AI51" s="25"/>
+      <c r="AJ51" s="25"/>
+      <c r="AK51" s="25"/>
       <c r="AL51" s="25"/>
-      <c r="AM51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN51" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO51" s="25" t="s">
-        <v>56</v>
-      </c>
+      <c r="AM51" s="25"/>
+      <c r="AN51" s="25"/>
+      <c r="AO51" s="25"/>
     </row>
     <row r="52" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E52" s="26">
-        <f>COUNT(E2:E46)</f>
-        <v>45</v>
-      </c>
-      <c r="F52" s="26">
-        <f t="shared" ref="F52:AO52" si="0">COUNT(F2:F46)</f>
-        <v>45</v>
-      </c>
-      <c r="G52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="H52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="J52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="K52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="L52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="M52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="N52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="O52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="P52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="Q52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="R52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="S52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="T52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="U52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="V52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="W52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="X52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="Y52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="Z52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AA52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AB52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AC52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AD52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AE52" s="26">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="AF52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AG52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AH52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AI52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AJ52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AK52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="26"/>
+      <c r="R52" s="26"/>
+      <c r="S52" s="26"/>
+      <c r="T52" s="26"/>
+      <c r="U52" s="26"/>
+      <c r="V52" s="26"/>
+      <c r="W52" s="26"/>
+      <c r="X52" s="26"/>
+      <c r="Y52" s="26"/>
+      <c r="Z52" s="26"/>
+      <c r="AA52" s="26"/>
+      <c r="AB52" s="26"/>
+      <c r="AC52" s="26"/>
+      <c r="AD52" s="26"/>
+      <c r="AE52" s="26"/>
+      <c r="AF52" s="26"/>
+      <c r="AG52" s="26"/>
+      <c r="AH52" s="26"/>
+      <c r="AI52" s="26"/>
+      <c r="AJ52" s="26"/>
+      <c r="AK52" s="26"/>
       <c r="AL52" s="26"/>
-      <c r="AM52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AN52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="AO52" s="26">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
+      <c r="AM52" s="26"/>
+      <c r="AN52" s="26"/>
+      <c r="AO52" s="26"/>
     </row>
     <row r="53" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="J53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="K53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="L53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="M53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="N53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="O53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="P53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="R53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="S53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="T53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="U53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="V53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="W53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="X53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AJ53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK53" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="25"/>
+      <c r="T53" s="25"/>
+      <c r="U53" s="25"/>
+      <c r="V53" s="25"/>
+      <c r="W53" s="25"/>
+      <c r="X53" s="25"/>
+      <c r="Y53" s="25"/>
+      <c r="Z53" s="25"/>
+      <c r="AA53" s="25"/>
+      <c r="AB53" s="25"/>
+      <c r="AC53" s="25"/>
+      <c r="AD53" s="25"/>
+      <c r="AE53" s="25"/>
+      <c r="AF53" s="25"/>
+      <c r="AG53" s="25"/>
+      <c r="AH53" s="25"/>
+      <c r="AI53" s="25"/>
+      <c r="AJ53" s="25"/>
+      <c r="AK53" s="25"/>
       <c r="AL53" s="25"/>
-      <c r="AM53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN53" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="AO53" s="25" t="s">
-        <v>55</v>
-      </c>
+      <c r="AM53" s="25"/>
+      <c r="AN53" s="25"/>
+      <c r="AO53" s="25"/>
     </row>
     <row r="54" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E54" s="27">
-        <f>AVERAGE(E2:E46)</f>
-        <v>71.888888888888886</v>
-      </c>
-      <c r="F54" s="27">
-        <f t="shared" ref="F54:AO54" si="1">AVERAGE(F2:F46)</f>
-        <v>78.022222222222226</v>
-      </c>
-      <c r="G54" s="27">
-        <f t="shared" si="1"/>
-        <v>153.6888888888889</v>
-      </c>
-      <c r="H54" s="27">
-        <f t="shared" si="1"/>
-        <v>88.511111111111106</v>
-      </c>
-      <c r="I54" s="27">
-        <f t="shared" si="1"/>
-        <v>135.60244444444444</v>
-      </c>
-      <c r="J54" s="27">
-        <f t="shared" si="1"/>
-        <v>9.0733333333333341</v>
-      </c>
-      <c r="K54" s="27">
-        <f t="shared" si="1"/>
-        <v>162.4</v>
-      </c>
-      <c r="L54" s="27">
-        <f t="shared" si="1"/>
-        <v>122.97777777777777</v>
-      </c>
-      <c r="M54" s="27">
-        <f t="shared" si="1"/>
-        <v>95.4</v>
-      </c>
-      <c r="N54" s="27">
-        <f t="shared" si="1"/>
-        <v>37.6</v>
-      </c>
-      <c r="O54" s="27">
-        <f t="shared" si="1"/>
-        <v>40.826666666666661</v>
-      </c>
-      <c r="P54" s="27">
-        <f t="shared" si="1"/>
-        <v>13.662222222222226</v>
-      </c>
-      <c r="Q54" s="27">
-        <f t="shared" si="1"/>
-        <v>235.06666666666666</v>
-      </c>
-      <c r="R54" s="27">
-        <f t="shared" si="1"/>
-        <v>1.1622222222222227</v>
-      </c>
-      <c r="S54" s="27">
-        <f t="shared" si="1"/>
-        <v>10.122444444444447</v>
-      </c>
-      <c r="T54" s="27">
-        <f t="shared" si="1"/>
-        <v>29.193777777777782</v>
-      </c>
-      <c r="U54" s="27">
-        <f t="shared" si="1"/>
-        <v>18.015333333333334</v>
-      </c>
-      <c r="V54" s="27">
-        <f t="shared" si="1"/>
-        <v>38.54955555555555</v>
-      </c>
-      <c r="W54" s="27">
-        <f t="shared" si="1"/>
-        <v>2.4091111111111112</v>
-      </c>
-      <c r="X54" s="27">
-        <f t="shared" si="1"/>
-        <v>31.271111111111104</v>
-      </c>
-      <c r="Y54" s="27">
-        <f t="shared" si="1"/>
-        <v>15.839999999999996</v>
-      </c>
-      <c r="Z54" s="27">
-        <f t="shared" si="1"/>
-        <v>139.05488888888891</v>
-      </c>
-      <c r="AA54" s="27">
-        <f t="shared" si="1"/>
-        <v>3.9893333333333318</v>
-      </c>
-      <c r="AB54" s="27">
-        <f t="shared" si="1"/>
-        <v>102.36555555555555</v>
-      </c>
-      <c r="AC54" s="27">
-        <f t="shared" si="1"/>
-        <v>98.009777777777785</v>
-      </c>
-      <c r="AD54" s="27">
-        <f t="shared" si="1"/>
-        <v>39.569333333333333</v>
-      </c>
-      <c r="AE54" s="27">
-        <f t="shared" si="1"/>
-        <v>14.045454545454545</v>
-      </c>
-      <c r="AF54" s="27">
-        <f t="shared" si="1"/>
-        <v>6.0666666666666664</v>
-      </c>
-      <c r="AG54" s="27">
-        <f t="shared" si="1"/>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="AH54" s="27">
-        <f t="shared" si="1"/>
-        <v>5.7555555555555555</v>
-      </c>
-      <c r="AI54" s="27">
-        <f t="shared" si="1"/>
-        <v>2.4222222222222221</v>
-      </c>
-      <c r="AJ54" s="27">
-        <f t="shared" si="1"/>
-        <v>2.2444444444444445</v>
-      </c>
-      <c r="AK54" s="27">
-        <f t="shared" si="1"/>
-        <v>2.4222222222222221</v>
-      </c>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+      <c r="O54" s="27"/>
+      <c r="P54" s="27"/>
+      <c r="Q54" s="27"/>
+      <c r="R54" s="27"/>
+      <c r="S54" s="27"/>
+      <c r="T54" s="27"/>
+      <c r="U54" s="27"/>
+      <c r="V54" s="27"/>
+      <c r="W54" s="27"/>
+      <c r="X54" s="27"/>
+      <c r="Y54" s="27"/>
+      <c r="Z54" s="27"/>
+      <c r="AA54" s="27"/>
+      <c r="AB54" s="27"/>
+      <c r="AC54" s="27"/>
+      <c r="AD54" s="27"/>
+      <c r="AE54" s="27"/>
+      <c r="AF54" s="27"/>
+      <c r="AG54" s="27"/>
+      <c r="AH54" s="27"/>
+      <c r="AI54" s="27"/>
+      <c r="AJ54" s="27"/>
+      <c r="AK54" s="27"/>
       <c r="AL54" s="27"/>
-      <c r="AM54" s="27">
-        <f t="shared" si="1"/>
-        <v>358.38980133333337</v>
-      </c>
-      <c r="AN54" s="27">
-        <f t="shared" si="1"/>
-        <v>98.92188588888888</v>
-      </c>
-      <c r="AO54" s="27">
-        <f t="shared" si="1"/>
-        <v>29.290757277448328</v>
-      </c>
+      <c r="AM54" s="27"/>
+      <c r="AN54" s="27"/>
+      <c r="AO54" s="27"/>
     </row>
     <row r="55" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="H55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="I55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="J55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="L55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="M55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="N55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="O55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="P55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="R55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="S55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="T55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="U55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="V55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="W55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="X55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AJ55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK55" s="25" t="s">
-        <v>57</v>
-      </c>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="25"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="25"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="25"/>
+      <c r="T55" s="25"/>
+      <c r="U55" s="25"/>
+      <c r="V55" s="25"/>
+      <c r="W55" s="25"/>
+      <c r="X55" s="25"/>
+      <c r="Y55" s="25"/>
+      <c r="Z55" s="25"/>
+      <c r="AA55" s="25"/>
+      <c r="AB55" s="25"/>
+      <c r="AC55" s="25"/>
+      <c r="AD55" s="25"/>
+      <c r="AE55" s="25"/>
+      <c r="AF55" s="25"/>
+      <c r="AG55" s="25"/>
+      <c r="AH55" s="25"/>
+      <c r="AI55" s="25"/>
+      <c r="AJ55" s="25"/>
+      <c r="AK55" s="25"/>
       <c r="AL55" s="25"/>
-      <c r="AM55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AN55" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO55" s="25" t="s">
-        <v>57</v>
-      </c>
+      <c r="AM55" s="25"/>
+      <c r="AN55" s="25"/>
+      <c r="AO55" s="25"/>
     </row>
     <row r="56" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E56" s="28">
-        <f>_xlfn.STDEV.S(E2:E46)</f>
-        <v>11.932046654859224</v>
-      </c>
-      <c r="F56" s="28">
-        <f t="shared" ref="F56:AO56" si="2">_xlfn.STDEV.S(F2:F46)</f>
-        <v>16.271124575440219</v>
-      </c>
-      <c r="G56" s="28">
-        <f t="shared" si="2"/>
-        <v>25.805057839520728</v>
-      </c>
-      <c r="H56" s="28">
-        <f t="shared" si="2"/>
-        <v>19.539729018105898</v>
-      </c>
-      <c r="I56" s="28">
-        <f t="shared" si="2"/>
-        <v>50.398835130638133</v>
-      </c>
-      <c r="J56" s="28">
-        <f t="shared" si="2"/>
-        <v>3.3913258335186423</v>
-      </c>
-      <c r="K56" s="28">
-        <f t="shared" si="2"/>
-        <v>49.288298445334512</v>
-      </c>
-      <c r="L56" s="28">
-        <f t="shared" si="2"/>
-        <v>43.83620799422701</v>
-      </c>
-      <c r="M56" s="28">
-        <f t="shared" si="2"/>
-        <v>44.595352387277472</v>
-      </c>
-      <c r="N56" s="28">
-        <f t="shared" si="2"/>
-        <v>8.1195611166658992</v>
-      </c>
-      <c r="O56" s="28">
-        <f t="shared" si="2"/>
-        <v>5.2672400915298043</v>
-      </c>
-      <c r="P56" s="28">
-        <f t="shared" si="2"/>
-        <v>1.8850233768611637</v>
-      </c>
-      <c r="Q56" s="28">
-        <f t="shared" si="2"/>
-        <v>82.509613764920502</v>
-      </c>
-      <c r="R56" s="28">
-        <f t="shared" si="2"/>
-        <v>0.36569292190485725</v>
-      </c>
-      <c r="S56" s="28">
-        <f t="shared" si="2"/>
-        <v>5.9807939407419886</v>
-      </c>
-      <c r="T56" s="28">
-        <f t="shared" si="2"/>
-        <v>61.792199062256181</v>
-      </c>
-      <c r="U56" s="28">
-        <f t="shared" si="2"/>
-        <v>8.1984792381381197</v>
-      </c>
-      <c r="V56" s="28">
-        <f t="shared" si="2"/>
-        <v>17.565551249735133</v>
-      </c>
-      <c r="W56" s="28">
-        <f t="shared" si="2"/>
-        <v>9.2530473658981958</v>
-      </c>
-      <c r="X56" s="28">
-        <f t="shared" si="2"/>
-        <v>6.6245281897939288</v>
-      </c>
-      <c r="Y56" s="28">
-        <f t="shared" si="2"/>
-        <v>15.493743605374755</v>
-      </c>
-      <c r="Z56" s="28">
-        <f t="shared" si="2"/>
-        <v>5.3908135758993758</v>
-      </c>
-      <c r="AA56" s="28">
-        <f t="shared" si="2"/>
-        <v>0.55386411198548402</v>
-      </c>
-      <c r="AB56" s="28">
-        <f t="shared" si="2"/>
-        <v>20.784183951390844</v>
-      </c>
-      <c r="AC56" s="28">
-        <f t="shared" si="2"/>
-        <v>52.450402740844289</v>
-      </c>
-      <c r="AD56" s="28">
-        <f t="shared" si="2"/>
-        <v>23.478455152833956</v>
-      </c>
-      <c r="AE56" s="28">
-        <f t="shared" si="2"/>
-        <v>1.4778133666749078</v>
-      </c>
-      <c r="AF56" s="28">
-        <f t="shared" si="2"/>
-        <v>4.9008348082935642</v>
-      </c>
-      <c r="AG56" s="28">
-        <f t="shared" si="2"/>
-        <v>1.3651506743346551</v>
-      </c>
-      <c r="AH56" s="28">
-        <f t="shared" si="2"/>
-        <v>9.9388026431657241</v>
-      </c>
-      <c r="AI56" s="28">
-        <f t="shared" si="2"/>
-        <v>1.864609255787302</v>
-      </c>
-      <c r="AJ56" s="28">
-        <f t="shared" si="2"/>
-        <v>4.2701690170698665</v>
-      </c>
-      <c r="AK56" s="28">
-        <f t="shared" si="2"/>
-        <v>2.0503756738803753</v>
-      </c>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="28"/>
+      <c r="P56" s="28"/>
+      <c r="Q56" s="28"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="28"/>
+      <c r="T56" s="28"/>
+      <c r="U56" s="28"/>
+      <c r="V56" s="28"/>
+      <c r="W56" s="28"/>
+      <c r="X56" s="28"/>
+      <c r="Y56" s="28"/>
+      <c r="Z56" s="28"/>
+      <c r="AA56" s="28"/>
+      <c r="AB56" s="28"/>
+      <c r="AC56" s="28"/>
+      <c r="AD56" s="28"/>
+      <c r="AE56" s="28"/>
+      <c r="AF56" s="28"/>
+      <c r="AG56" s="28"/>
+      <c r="AH56" s="28"/>
+      <c r="AI56" s="28"/>
+      <c r="AJ56" s="28"/>
+      <c r="AK56" s="28"/>
       <c r="AL56" s="28"/>
-      <c r="AM56" s="28">
-        <f t="shared" si="2"/>
-        <v>229.33400622484342</v>
-      </c>
-      <c r="AN56" s="28">
-        <f t="shared" si="2"/>
-        <v>31.477188708761162</v>
-      </c>
-      <c r="AO56" s="28">
-        <f t="shared" si="2"/>
-        <v>28.501699983338664</v>
-      </c>
+      <c r="AM56" s="28"/>
+      <c r="AN56" s="28"/>
+      <c r="AO56" s="28"/>
     </row>
     <row r="57" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="G57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="I57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="K57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="L57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="M57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="N57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="O57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="P57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="R57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="S57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="T57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="U57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="V57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="W57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="X57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK57" s="25" t="s">
-        <v>58</v>
-      </c>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="25"/>
+      <c r="K57" s="25"/>
+      <c r="L57" s="25"/>
+      <c r="M57" s="25"/>
+      <c r="N57" s="25"/>
+      <c r="O57" s="25"/>
+      <c r="P57" s="25"/>
+      <c r="Q57" s="25"/>
+      <c r="R57" s="25"/>
+      <c r="S57" s="25"/>
+      <c r="T57" s="25"/>
+      <c r="U57" s="25"/>
+      <c r="V57" s="25"/>
+      <c r="W57" s="25"/>
+      <c r="X57" s="25"/>
+      <c r="Y57" s="25"/>
+      <c r="Z57" s="25"/>
+      <c r="AA57" s="25"/>
+      <c r="AB57" s="25"/>
+      <c r="AC57" s="25"/>
+      <c r="AD57" s="25"/>
+      <c r="AE57" s="25"/>
+      <c r="AF57" s="25"/>
+      <c r="AG57" s="25"/>
+      <c r="AH57" s="25"/>
+      <c r="AI57" s="25"/>
+      <c r="AJ57" s="25"/>
+      <c r="AK57" s="25"/>
       <c r="AL57" s="25"/>
-      <c r="AM57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN57" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO57" s="25" t="s">
-        <v>58</v>
-      </c>
+      <c r="AM57" s="25"/>
+      <c r="AN57" s="25"/>
+      <c r="AO57" s="25"/>
     </row>
     <row r="58" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E58" s="26">
-        <f>MIN(E2:E46)</f>
-        <v>38</v>
-      </c>
-      <c r="F58" s="26">
-        <f t="shared" ref="F58:AO58" si="3">MIN(F2:F46)</f>
-        <v>40</v>
-      </c>
-      <c r="G58" s="26">
-        <f t="shared" si="3"/>
-        <v>115</v>
-      </c>
-      <c r="H58" s="26">
-        <f t="shared" si="3"/>
-        <v>32</v>
-      </c>
-      <c r="I58" s="26">
-        <f t="shared" si="3"/>
-        <v>82.61</v>
-      </c>
-      <c r="J58" s="26">
-        <f t="shared" si="3"/>
-        <v>4.8</v>
-      </c>
-      <c r="K58" s="26">
-        <f t="shared" si="3"/>
-        <v>85</v>
-      </c>
-      <c r="L58" s="26">
-        <f t="shared" si="3"/>
-        <v>57</v>
-      </c>
-      <c r="M58" s="26">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="N58" s="26">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="O58" s="26">
-        <f t="shared" si="3"/>
-        <v>25.2</v>
-      </c>
-      <c r="P58" s="26">
-        <f t="shared" si="3"/>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="Q58" s="26">
-        <f t="shared" si="3"/>
-        <v>113</v>
-      </c>
-      <c r="R58" s="26">
-        <f t="shared" si="3"/>
-        <v>0.89</v>
-      </c>
-      <c r="S58" s="26">
-        <f t="shared" si="3"/>
-        <v>3.76</v>
-      </c>
-      <c r="T58" s="26">
-        <f t="shared" si="3"/>
-        <v>0.36</v>
-      </c>
-      <c r="U58" s="26">
-        <f t="shared" si="3"/>
-        <v>6.18</v>
-      </c>
-      <c r="V58" s="26">
-        <f t="shared" si="3"/>
-        <v>13.23</v>
-      </c>
-      <c r="W58" s="26">
-        <f t="shared" si="3"/>
-        <v>0.53</v>
-      </c>
-      <c r="X58" s="26">
-        <f t="shared" si="3"/>
-        <v>21.8</v>
-      </c>
-      <c r="Y58" s="26">
-        <f t="shared" si="3"/>
-        <v>8.4</v>
-      </c>
-      <c r="Z58" s="26">
-        <f t="shared" si="3"/>
-        <v>125.07</v>
-      </c>
-      <c r="AA58" s="26">
-        <f t="shared" si="3"/>
-        <v>2.87</v>
-      </c>
-      <c r="AB58" s="26">
-        <f t="shared" si="3"/>
-        <v>11.09</v>
-      </c>
-      <c r="AC58" s="26">
-        <f t="shared" si="3"/>
-        <v>53.41</v>
-      </c>
-      <c r="AD58" s="26">
-        <f t="shared" si="3"/>
-        <v>11.61</v>
-      </c>
-      <c r="AE58" s="26">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="AF58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK58" s="26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+      <c r="L58" s="26"/>
+      <c r="M58" s="26"/>
+      <c r="N58" s="26"/>
+      <c r="O58" s="26"/>
+      <c r="P58" s="26"/>
+      <c r="Q58" s="26"/>
+      <c r="R58" s="26"/>
+      <c r="S58" s="26"/>
+      <c r="T58" s="26"/>
+      <c r="U58" s="26"/>
+      <c r="V58" s="26"/>
+      <c r="W58" s="26"/>
+      <c r="X58" s="26"/>
+      <c r="Y58" s="26"/>
+      <c r="Z58" s="26"/>
+      <c r="AA58" s="26"/>
+      <c r="AB58" s="26"/>
+      <c r="AC58" s="26"/>
+      <c r="AD58" s="26"/>
+      <c r="AE58" s="26"/>
+      <c r="AF58" s="26"/>
+      <c r="AG58" s="26"/>
+      <c r="AH58" s="26"/>
+      <c r="AI58" s="26"/>
+      <c r="AJ58" s="26"/>
+      <c r="AK58" s="26"/>
       <c r="AL58" s="26"/>
-      <c r="AM58" s="26">
-        <f t="shared" si="3"/>
-        <v>103.85811</v>
-      </c>
-      <c r="AN58" s="26">
-        <f t="shared" si="3"/>
-        <v>43.984210000000004</v>
-      </c>
-      <c r="AO58" s="26">
-        <f t="shared" si="3"/>
-        <v>0.103523913162359</v>
-      </c>
+      <c r="AM58" s="26"/>
+      <c r="AN58" s="26"/>
+      <c r="AO58" s="26"/>
     </row>
     <row r="59" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="G59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="I59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="J59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="K59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="M59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="N59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="O59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="P59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="R59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="S59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="T59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="U59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="V59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="W59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="X59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK59" s="25" t="s">
-        <v>59</v>
-      </c>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="25"/>
+      <c r="J59" s="25"/>
+      <c r="K59" s="25"/>
+      <c r="L59" s="25"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="25"/>
+      <c r="O59" s="25"/>
+      <c r="P59" s="25"/>
+      <c r="Q59" s="25"/>
+      <c r="R59" s="25"/>
+      <c r="S59" s="25"/>
+      <c r="T59" s="25"/>
+      <c r="U59" s="25"/>
+      <c r="V59" s="25"/>
+      <c r="W59" s="25"/>
+      <c r="X59" s="25"/>
+      <c r="Y59" s="25"/>
+      <c r="Z59" s="25"/>
+      <c r="AA59" s="25"/>
+      <c r="AB59" s="25"/>
+      <c r="AC59" s="25"/>
+      <c r="AD59" s="25"/>
+      <c r="AE59" s="25"/>
+      <c r="AF59" s="25"/>
+      <c r="AG59" s="25"/>
+      <c r="AH59" s="25"/>
+      <c r="AI59" s="25"/>
+      <c r="AJ59" s="25"/>
+      <c r="AK59" s="25"/>
       <c r="AL59" s="25"/>
-      <c r="AM59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN59" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO59" s="25" t="s">
-        <v>59</v>
-      </c>
+      <c r="AM59" s="25"/>
+      <c r="AN59" s="25"/>
+      <c r="AO59" s="25"/>
     </row>
     <row r="60" spans="5:41" x14ac:dyDescent="0.25">
-      <c r="E60" s="27">
-        <f>MAX(E2:E46)</f>
-        <v>90</v>
-      </c>
-      <c r="F60" s="27">
-        <f t="shared" ref="F60:AO60" si="4">MAX(F2:F46)</f>
-        <v>126</v>
-      </c>
-      <c r="G60" s="27">
-        <f t="shared" si="4"/>
-        <v>216</v>
-      </c>
-      <c r="H60" s="27">
-        <f t="shared" si="4"/>
-        <v>125</v>
-      </c>
-      <c r="I60" s="27">
-        <f t="shared" si="4"/>
-        <v>359.42</v>
-      </c>
-      <c r="J60" s="27">
-        <f t="shared" si="4"/>
-        <v>16.7</v>
-      </c>
-      <c r="K60" s="27">
-        <f t="shared" si="4"/>
-        <v>342</v>
-      </c>
-      <c r="L60" s="27">
-        <f t="shared" si="4"/>
-        <v>232</v>
-      </c>
-      <c r="M60" s="27">
-        <f t="shared" si="4"/>
-        <v>254</v>
-      </c>
-      <c r="N60" s="27">
-        <f t="shared" si="4"/>
-        <v>58</v>
-      </c>
-      <c r="O60" s="27">
-        <f t="shared" si="4"/>
-        <v>51.4</v>
-      </c>
-      <c r="P60" s="27">
-        <f t="shared" si="4"/>
-        <v>17.8</v>
-      </c>
-      <c r="Q60" s="27">
-        <f t="shared" si="4"/>
-        <v>622</v>
-      </c>
-      <c r="R60" s="27">
-        <f t="shared" si="4"/>
-        <v>3.08</v>
-      </c>
-      <c r="S60" s="27">
-        <f t="shared" si="4"/>
-        <v>41.9</v>
-      </c>
-      <c r="T60" s="27">
-        <f t="shared" si="4"/>
-        <v>376.72</v>
-      </c>
-      <c r="U60" s="27">
-        <f t="shared" si="4"/>
-        <v>46.35</v>
-      </c>
-      <c r="V60" s="27">
-        <f t="shared" si="4"/>
-        <v>99.19</v>
-      </c>
-      <c r="W60" s="27">
-        <f t="shared" si="4"/>
-        <v>63</v>
-      </c>
-      <c r="X60" s="27">
-        <f t="shared" si="4"/>
-        <v>52.9</v>
-      </c>
-      <c r="Y60" s="27">
-        <f t="shared" si="4"/>
-        <v>104</v>
-      </c>
-      <c r="Z60" s="27">
-        <f t="shared" si="4"/>
-        <v>164.34</v>
-      </c>
-      <c r="AA60" s="27">
-        <f t="shared" si="4"/>
-        <v>5.81</v>
-      </c>
-      <c r="AB60" s="27">
-        <f t="shared" si="4"/>
-        <v>143.99</v>
-      </c>
-      <c r="AC60" s="27">
-        <f t="shared" si="4"/>
-        <v>411.28</v>
-      </c>
-      <c r="AD60" s="27">
-        <f t="shared" si="4"/>
-        <v>130.38999999999999</v>
-      </c>
-      <c r="AE60" s="27">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="AF60" s="27">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="AG60" s="27">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="AH60" s="27">
-        <f t="shared" si="4"/>
-        <v>42</v>
-      </c>
-      <c r="AI60" s="27">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="AJ60" s="27">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-      <c r="AK60" s="27">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="27"/>
+      <c r="N60" s="27"/>
+      <c r="O60" s="27"/>
+      <c r="P60" s="27"/>
+      <c r="Q60" s="27"/>
+      <c r="R60" s="27"/>
+      <c r="S60" s="27"/>
+      <c r="T60" s="27"/>
+      <c r="U60" s="27"/>
+      <c r="V60" s="27"/>
+      <c r="W60" s="27"/>
+      <c r="X60" s="27"/>
+      <c r="Y60" s="27"/>
+      <c r="Z60" s="27"/>
+      <c r="AA60" s="27"/>
+      <c r="AB60" s="27"/>
+      <c r="AC60" s="27"/>
+      <c r="AD60" s="27"/>
+      <c r="AE60" s="27"/>
+      <c r="AF60" s="27"/>
+      <c r="AG60" s="27"/>
+      <c r="AH60" s="27"/>
+      <c r="AI60" s="27"/>
+      <c r="AJ60" s="27"/>
+      <c r="AK60" s="27"/>
       <c r="AL60" s="27"/>
-      <c r="AM60" s="27">
-        <f t="shared" si="4"/>
-        <v>1220.874</v>
-      </c>
-      <c r="AN60" s="27">
-        <f t="shared" si="4"/>
-        <v>173.62785000000002</v>
-      </c>
-      <c r="AO60" s="27">
-        <f t="shared" si="4"/>
-        <v>114.28888038272601</v>
-      </c>
+      <c r="AM60" s="27"/>
+      <c r="AN60" s="27"/>
+      <c r="AO60" s="27"/>
     </row>
     <row r="61" spans="5:41" x14ac:dyDescent="0.25">
       <c r="E61" s="6"/>

</xml_diff>